<commit_message>
Updated config.json to removed cases in dataset
</commit_message>
<xml_diff>
--- a/data/feature_selection/features.xlsx
+++ b/data/feature_selection/features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\HiwiJob\PredMSiamNN\data\feature_selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5525F1-8F2B-47CC-9A5A-8DA119F72E27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5BA58F-1A27-4030-B7A4-64AEFDCD5FD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>a_15_1_x</t>
   </si>
@@ -157,9 +157,6 @@
     <t>txt15_i1_lightbarrier_failure_mode_2</t>
   </si>
   <si>
-    <t>txt15_i3_lightbarrier_failure_mode_1</t>
-  </si>
-  <si>
     <t>txt15_i3_lightbarrier_failure_mode_2</t>
   </si>
   <si>
@@ -227,9 +224,6 @@
   </si>
   <si>
     <t>txt18_pneumatic_leakage_failure_mode_2_faulty</t>
-  </si>
-  <si>
-    <t>txt18_pneumatic_leakage_failure_mode_3_faulty</t>
   </si>
   <si>
     <t>txt18_transport_failure_mode_wout_workpiece</t>
@@ -245,7 +239,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,8 +252,15 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,49 +269,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -342,43 +349,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -681,15 +665,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP33"/>
+  <dimension ref="A1:AP31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.28515625" customWidth="1"/>
+    <col min="1" max="1" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.25">
@@ -818,144 +802,144 @@
       </c>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1</v>
-      </c>
-      <c r="J2" s="3">
-        <v>1</v>
-      </c>
-      <c r="K2" s="3">
-        <v>1</v>
-      </c>
-      <c r="L2" s="3">
-        <v>1</v>
-      </c>
-      <c r="M2" s="3">
-        <v>1</v>
-      </c>
-      <c r="N2" s="3">
-        <v>1</v>
-      </c>
-      <c r="O2" s="3">
-        <v>1</v>
-      </c>
-      <c r="P2" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>1</v>
-      </c>
-      <c r="R2" s="3">
-        <v>1</v>
-      </c>
-      <c r="S2" s="3">
-        <v>1</v>
-      </c>
-      <c r="T2" s="3">
-        <v>1</v>
-      </c>
-      <c r="U2" s="3">
-        <v>1</v>
-      </c>
-      <c r="V2" s="3">
-        <v>1</v>
-      </c>
-      <c r="W2" s="3">
-        <v>1</v>
-      </c>
-      <c r="X2" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AO2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AP2" s="3">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1</v>
+      </c>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>1</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="2">
+        <v>1</v>
+      </c>
+      <c r="U2" s="2">
+        <v>1</v>
+      </c>
+      <c r="V2" s="2">
+        <v>1</v>
+      </c>
+      <c r="W2" s="2">
+        <v>1</v>
+      </c>
+      <c r="X2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3">
@@ -976,13 +960,13 @@
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3" s="5">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5">
-        <v>0</v>
-      </c>
-      <c r="M3" s="5">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
         <v>1</v>
       </c>
       <c r="N3">
@@ -1074,16 +1058,16 @@
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
@@ -1104,13 +1088,13 @@
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4" s="5">
-        <v>1</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0</v>
-      </c>
-      <c r="M4" s="5">
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
         <v>1</v>
       </c>
       <c r="N4">
@@ -1202,16 +1186,16 @@
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
@@ -1232,13 +1216,13 @@
       <c r="J5">
         <v>0</v>
       </c>
-      <c r="K5" s="5">
-        <v>1</v>
-      </c>
-      <c r="L5" s="5">
-        <v>0</v>
-      </c>
-      <c r="M5" s="5">
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
         <v>1</v>
       </c>
       <c r="N5">
@@ -1330,16 +1314,16 @@
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
@@ -1360,13 +1344,13 @@
       <c r="J6">
         <v>0</v>
       </c>
-      <c r="K6" s="5">
-        <v>0</v>
-      </c>
-      <c r="L6" s="5">
-        <v>1</v>
-      </c>
-      <c r="M6" s="5">
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+      <c r="M6" s="4">
         <v>1</v>
       </c>
       <c r="N6">
@@ -1458,17 +1442,17 @@
       </c>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1488,13 +1472,13 @@
       <c r="J7">
         <v>0</v>
       </c>
-      <c r="K7" s="5">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5">
-        <v>1</v>
-      </c>
-      <c r="M7" s="5">
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
         <v>1</v>
       </c>
       <c r="N7">
@@ -1586,16 +1570,16 @@
       </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
         <v>1</v>
       </c>
       <c r="E8">
@@ -1616,13 +1600,13 @@
       <c r="J8">
         <v>0</v>
       </c>
-      <c r="K8" s="5">
-        <v>0</v>
-      </c>
-      <c r="L8" s="5">
-        <v>0</v>
-      </c>
-      <c r="M8" s="5">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
         <v>1</v>
       </c>
       <c r="N8">
@@ -1714,16 +1698,16 @@
       </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
         <v>1</v>
       </c>
       <c r="E9">
@@ -1744,13 +1728,13 @@
       <c r="J9">
         <v>0</v>
       </c>
-      <c r="K9" s="5">
-        <v>0</v>
-      </c>
-      <c r="L9" s="5">
-        <v>0</v>
-      </c>
-      <c r="M9" s="5">
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
         <v>1</v>
       </c>
       <c r="N9">
@@ -1842,17 +1826,17 @@
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1</v>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1863,8 +1847,8 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10">
-        <v>0</v>
+      <c r="H10" s="5">
+        <v>1</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1872,26 +1856,26 @@
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10" s="5">
-        <v>0</v>
-      </c>
-      <c r="L10" s="5">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>1</v>
+      </c>
+      <c r="O10" s="5">
+        <v>1</v>
+      </c>
+      <c r="P10" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>1</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -1970,7 +1954,7 @@
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B11">
@@ -1991,7 +1975,7 @@
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>1</v>
       </c>
       <c r="I11">
@@ -2009,16 +1993,16 @@
       <c r="M11">
         <v>0</v>
       </c>
-      <c r="N11" s="6">
-        <v>1</v>
-      </c>
-      <c r="O11" s="6">
-        <v>1</v>
-      </c>
-      <c r="P11" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="6">
+      <c r="N11" s="5">
+        <v>1</v>
+      </c>
+      <c r="O11" s="5">
+        <v>1</v>
+      </c>
+      <c r="P11" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="5">
         <v>1</v>
       </c>
       <c r="R11">
@@ -2098,7 +2082,7 @@
       </c>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B12">
@@ -2119,7 +2103,7 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>1</v>
       </c>
       <c r="I12">
@@ -2137,16 +2121,16 @@
       <c r="M12">
         <v>0</v>
       </c>
-      <c r="N12" s="6">
-        <v>1</v>
-      </c>
-      <c r="O12" s="6">
-        <v>1</v>
-      </c>
-      <c r="P12" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="6">
+      <c r="N12" s="5">
+        <v>1</v>
+      </c>
+      <c r="O12" s="5">
+        <v>1</v>
+      </c>
+      <c r="P12" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="5">
         <v>1</v>
       </c>
       <c r="R12">
@@ -2226,7 +2210,7 @@
       </c>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B13">
@@ -2238,17 +2222,17 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6">
-        <v>1</v>
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -2265,17 +2249,17 @@
       <c r="M13">
         <v>0</v>
       </c>
-      <c r="N13" s="6">
-        <v>1</v>
-      </c>
-      <c r="O13" s="6">
-        <v>1</v>
-      </c>
-      <c r="P13" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="6">
-        <v>1</v>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -2286,8 +2270,8 @@
       <c r="T13">
         <v>0</v>
       </c>
-      <c r="U13">
-        <v>0</v>
+      <c r="U13" s="6">
+        <v>1</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -2354,7 +2338,7 @@
       </c>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B14">
@@ -2366,13 +2350,13 @@
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" s="9">
-        <v>1</v>
-      </c>
-      <c r="F14" s="9">
-        <v>1</v>
-      </c>
-      <c r="G14" s="9">
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6">
         <v>1</v>
       </c>
       <c r="H14">
@@ -2414,7 +2398,7 @@
       <c r="T14">
         <v>0</v>
       </c>
-      <c r="U14" s="9">
+      <c r="U14" s="6">
         <v>1</v>
       </c>
       <c r="V14">
@@ -2482,7 +2466,7 @@
       </c>
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B15">
@@ -2494,13 +2478,13 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15" s="9">
-        <v>1</v>
-      </c>
-      <c r="F15" s="9">
-        <v>1</v>
-      </c>
-      <c r="G15" s="9">
+      <c r="E15" s="6">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6">
         <v>1</v>
       </c>
       <c r="H15">
@@ -2542,7 +2526,7 @@
       <c r="T15">
         <v>0</v>
       </c>
-      <c r="U15" s="9">
+      <c r="U15" s="6">
         <v>1</v>
       </c>
       <c r="V15">
@@ -2610,7 +2594,7 @@
       </c>
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B16">
@@ -2622,14 +2606,14 @@
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16" s="9">
-        <v>1</v>
-      </c>
-      <c r="F16" s="9">
-        <v>1</v>
-      </c>
-      <c r="G16" s="9">
-        <v>1</v>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -2661,17 +2645,17 @@
       <c r="Q16">
         <v>0</v>
       </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16" s="9">
-        <v>1</v>
+      <c r="R16" s="10">
+        <v>1</v>
+      </c>
+      <c r="S16" s="10">
+        <v>0</v>
+      </c>
+      <c r="T16" s="10">
+        <v>1</v>
+      </c>
+      <c r="U16" s="10">
+        <v>0</v>
       </c>
       <c r="V16">
         <v>0</v>
@@ -2738,7 +2722,7 @@
       </c>
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B17">
@@ -2789,17 +2773,17 @@
       <c r="Q17">
         <v>0</v>
       </c>
-      <c r="R17" s="16">
-        <v>1</v>
-      </c>
-      <c r="S17" s="16">
-        <v>0</v>
-      </c>
-      <c r="T17" s="16">
-        <v>1</v>
-      </c>
-      <c r="U17" s="16">
-        <v>0</v>
+      <c r="R17" s="10">
+        <v>0</v>
+      </c>
+      <c r="S17" s="10">
+        <v>1</v>
+      </c>
+      <c r="T17" s="10">
+        <v>0</v>
+      </c>
+      <c r="U17" s="10">
+        <v>1</v>
       </c>
       <c r="V17">
         <v>0</v>
@@ -2866,7 +2850,7 @@
       </c>
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B18">
@@ -2878,14 +2862,14 @@
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
+      <c r="E18" s="6">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -2917,16 +2901,16 @@
       <c r="Q18">
         <v>0</v>
       </c>
-      <c r="R18" s="16">
-        <v>0</v>
-      </c>
-      <c r="S18" s="16">
-        <v>1</v>
-      </c>
-      <c r="T18" s="16">
-        <v>0</v>
-      </c>
-      <c r="U18" s="16">
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18" s="6">
         <v>1</v>
       </c>
       <c r="V18">
@@ -2994,7 +2978,7 @@
       </c>
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B19">
@@ -3006,13 +2990,13 @@
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19" s="9">
-        <v>1</v>
-      </c>
-      <c r="F19" s="9">
-        <v>1</v>
-      </c>
-      <c r="G19" s="9">
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6">
         <v>1</v>
       </c>
       <c r="H19">
@@ -3054,7 +3038,7 @@
       <c r="T19">
         <v>0</v>
       </c>
-      <c r="U19" s="9">
+      <c r="U19" s="6">
         <v>1</v>
       </c>
       <c r="V19">
@@ -3122,7 +3106,7 @@
       </c>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B20">
@@ -3134,13 +3118,13 @@
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20" s="9">
-        <v>1</v>
-      </c>
-      <c r="F20" s="9">
-        <v>1</v>
-      </c>
-      <c r="G20" s="9">
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1</v>
+      </c>
+      <c r="G20" s="6">
         <v>1</v>
       </c>
       <c r="H20">
@@ -3182,7 +3166,7 @@
       <c r="T20">
         <v>0</v>
       </c>
-      <c r="U20" s="9">
+      <c r="U20" s="6">
         <v>1</v>
       </c>
       <c r="V20">
@@ -3250,7 +3234,7 @@
       </c>
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B21">
@@ -3262,20 +3246,20 @@
       <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21" s="9">
-        <v>1</v>
-      </c>
-      <c r="F21" s="9">
-        <v>1</v>
-      </c>
-      <c r="G21" s="9">
-        <v>1</v>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
-      <c r="I21">
-        <v>0</v>
+      <c r="I21" s="9">
+        <v>1</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -3310,38 +3294,38 @@
       <c r="T21">
         <v>0</v>
       </c>
-      <c r="U21" s="9">
-        <v>1</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <v>0</v>
-      </c>
-      <c r="X21">
-        <v>0</v>
-      </c>
-      <c r="Y21">
-        <v>0</v>
-      </c>
-      <c r="Z21">
-        <v>0</v>
-      </c>
-      <c r="AA21">
-        <v>0</v>
-      </c>
-      <c r="AB21">
-        <v>0</v>
-      </c>
-      <c r="AC21">
-        <v>0</v>
-      </c>
-      <c r="AD21">
-        <v>0</v>
-      </c>
-      <c r="AE21">
-        <v>0</v>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21" s="9">
+        <v>1</v>
+      </c>
+      <c r="W21" s="9">
+        <v>1</v>
+      </c>
+      <c r="X21" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE21" s="9">
+        <v>1</v>
       </c>
       <c r="AF21">
         <v>0</v>
@@ -3378,7 +3362,7 @@
       </c>
     </row>
     <row r="22" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B22">
@@ -3402,8 +3386,8 @@
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="I22" s="10">
-        <v>1</v>
+      <c r="I22" s="9">
+        <v>0</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -3441,34 +3425,34 @@
       <c r="U22">
         <v>0</v>
       </c>
-      <c r="V22" s="10">
-        <v>1</v>
-      </c>
-      <c r="W22" s="10">
-        <v>1</v>
-      </c>
-      <c r="X22" s="10">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="10">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="10">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="10">
-        <v>1</v>
-      </c>
-      <c r="AD22" s="10">
-        <v>1</v>
-      </c>
-      <c r="AE22" s="10">
+      <c r="V22" s="9">
+        <v>0</v>
+      </c>
+      <c r="W22" s="9">
+        <v>1</v>
+      </c>
+      <c r="X22" s="9">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="9">
         <v>1</v>
       </c>
       <c r="AF22">
@@ -3477,10 +3461,10 @@
       <c r="AG22">
         <v>0</v>
       </c>
-      <c r="AH22" s="10">
-        <v>0</v>
-      </c>
-      <c r="AI22" s="10">
+      <c r="AH22">
+        <v>0</v>
+      </c>
+      <c r="AI22">
         <v>0</v>
       </c>
       <c r="AJ22">
@@ -3506,7 +3490,7 @@
       </c>
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B23">
@@ -3530,7 +3514,7 @@
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="9">
         <v>0</v>
       </c>
       <c r="J23">
@@ -3569,34 +3553,34 @@
       <c r="U23">
         <v>0</v>
       </c>
-      <c r="V23" s="10">
-        <v>0</v>
-      </c>
-      <c r="W23" s="10">
-        <v>1</v>
-      </c>
-      <c r="X23" s="10">
-        <v>1</v>
-      </c>
-      <c r="Y23" s="10">
-        <v>1</v>
-      </c>
-      <c r="Z23" s="10">
-        <v>1</v>
-      </c>
-      <c r="AA23" s="10">
-        <v>1</v>
-      </c>
-      <c r="AB23" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="10">
-        <v>0</v>
-      </c>
-      <c r="AD23" s="10">
-        <v>0</v>
-      </c>
-      <c r="AE23" s="10">
+      <c r="V23" s="9">
+        <v>0</v>
+      </c>
+      <c r="W23" s="9">
+        <v>1</v>
+      </c>
+      <c r="X23" s="9">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="9">
         <v>1</v>
       </c>
       <c r="AF23">
@@ -3605,10 +3589,10 @@
       <c r="AG23">
         <v>0</v>
       </c>
-      <c r="AH23" s="10">
-        <v>0</v>
-      </c>
-      <c r="AI23" s="10">
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
         <v>0</v>
       </c>
       <c r="AJ23">
@@ -3634,7 +3618,7 @@
       </c>
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B24">
@@ -3658,8 +3642,8 @@
       <c r="H24">
         <v>0</v>
       </c>
-      <c r="I24" s="10">
-        <v>0</v>
+      <c r="I24" s="9">
+        <v>1</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -3697,34 +3681,34 @@
       <c r="U24">
         <v>0</v>
       </c>
-      <c r="V24" s="10">
-        <v>0</v>
-      </c>
-      <c r="W24" s="10">
-        <v>1</v>
-      </c>
-      <c r="X24" s="10">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="10">
-        <v>1</v>
-      </c>
-      <c r="Z24" s="10">
-        <v>1</v>
-      </c>
-      <c r="AA24" s="10">
-        <v>1</v>
-      </c>
-      <c r="AB24" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC24" s="10">
-        <v>0</v>
-      </c>
-      <c r="AD24" s="10">
-        <v>0</v>
-      </c>
-      <c r="AE24" s="10">
+      <c r="V24" s="9">
+        <v>0</v>
+      </c>
+      <c r="W24" s="9">
+        <v>0</v>
+      </c>
+      <c r="X24" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE24" s="9">
         <v>1</v>
       </c>
       <c r="AF24">
@@ -3733,10 +3717,10 @@
       <c r="AG24">
         <v>0</v>
       </c>
-      <c r="AH24" s="10">
-        <v>0</v>
-      </c>
-      <c r="AI24" s="10">
+      <c r="AH24">
+        <v>0</v>
+      </c>
+      <c r="AI24">
         <v>0</v>
       </c>
       <c r="AJ24">
@@ -3762,7 +3746,7 @@
       </c>
     </row>
     <row r="25" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B25">
@@ -3786,7 +3770,7 @@
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="9">
         <v>1</v>
       </c>
       <c r="J25">
@@ -3825,34 +3809,34 @@
       <c r="U25">
         <v>0</v>
       </c>
-      <c r="V25" s="10">
-        <v>0</v>
-      </c>
-      <c r="W25" s="10">
-        <v>0</v>
-      </c>
-      <c r="X25" s="10">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="10">
-        <v>1</v>
-      </c>
-      <c r="Z25" s="10">
-        <v>1</v>
-      </c>
-      <c r="AA25" s="10">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="10">
-        <v>1</v>
-      </c>
-      <c r="AC25" s="10">
-        <v>1</v>
-      </c>
-      <c r="AD25" s="10">
-        <v>1</v>
-      </c>
-      <c r="AE25" s="10">
+      <c r="V25" s="9">
+        <v>1</v>
+      </c>
+      <c r="W25" s="9">
+        <v>1</v>
+      </c>
+      <c r="X25" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD25" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE25" s="9">
         <v>1</v>
       </c>
       <c r="AF25">
@@ -3861,10 +3845,10 @@
       <c r="AG25">
         <v>0</v>
       </c>
-      <c r="AH25" s="10">
-        <v>0</v>
-      </c>
-      <c r="AI25" s="10">
+      <c r="AH25">
+        <v>0</v>
+      </c>
+      <c r="AI25">
         <v>0</v>
       </c>
       <c r="AJ25">
@@ -3890,7 +3874,7 @@
       </c>
     </row>
     <row r="26" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B26">
@@ -3914,11 +3898,11 @@
       <c r="H26">
         <v>0</v>
       </c>
-      <c r="I26" s="10">
-        <v>1</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26" s="8">
+        <v>1</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -3953,53 +3937,53 @@
       <c r="U26">
         <v>0</v>
       </c>
-      <c r="V26" s="10">
-        <v>1</v>
-      </c>
-      <c r="W26" s="10">
-        <v>1</v>
-      </c>
-      <c r="X26" s="10">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="10">
-        <v>1</v>
-      </c>
-      <c r="AA26" s="10">
-        <v>1</v>
-      </c>
-      <c r="AB26" s="10">
-        <v>1</v>
-      </c>
-      <c r="AC26" s="10">
-        <v>1</v>
-      </c>
-      <c r="AD26" s="10">
-        <v>1</v>
-      </c>
-      <c r="AE26" s="10">
-        <v>1</v>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AB26">
+        <v>0</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <v>0</v>
       </c>
       <c r="AF26">
         <v>0</v>
       </c>
-      <c r="AG26">
-        <v>0</v>
-      </c>
-      <c r="AH26" s="10">
-        <v>1</v>
-      </c>
-      <c r="AI26" s="10">
-        <v>1</v>
-      </c>
-      <c r="AJ26">
-        <v>0</v>
-      </c>
-      <c r="AK26">
-        <v>0</v>
+      <c r="AG26" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="8">
+        <v>1</v>
+      </c>
+      <c r="AK26" s="8">
+        <v>1</v>
       </c>
       <c r="AL26">
         <v>0</v>
@@ -4018,7 +4002,7 @@
       </c>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B27">
@@ -4045,7 +4029,7 @@
       <c r="I27">
         <v>0</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J27" s="8">
         <v>1</v>
       </c>
       <c r="K27">
@@ -4114,19 +4098,19 @@
       <c r="AF27">
         <v>0</v>
       </c>
-      <c r="AG27" s="11">
-        <v>0</v>
-      </c>
-      <c r="AH27" s="11">
-        <v>0</v>
-      </c>
-      <c r="AI27" s="11">
-        <v>0</v>
-      </c>
-      <c r="AJ27" s="11">
-        <v>1</v>
-      </c>
-      <c r="AK27" s="11">
+      <c r="AG27" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="8">
+        <v>1</v>
+      </c>
+      <c r="AK27" s="8">
         <v>1</v>
       </c>
       <c r="AL27">
@@ -4146,7 +4130,7 @@
       </c>
     </row>
     <row r="28" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B28">
@@ -4173,7 +4157,7 @@
       <c r="I28">
         <v>0</v>
       </c>
-      <c r="J28" s="11">
+      <c r="J28" s="8">
         <v>1</v>
       </c>
       <c r="K28">
@@ -4242,19 +4226,19 @@
       <c r="AF28">
         <v>0</v>
       </c>
-      <c r="AG28" s="11">
-        <v>0</v>
-      </c>
-      <c r="AH28" s="11">
-        <v>0</v>
-      </c>
-      <c r="AI28" s="11">
-        <v>0</v>
-      </c>
-      <c r="AJ28" s="11">
-        <v>1</v>
-      </c>
-      <c r="AK28" s="11">
+      <c r="AG28" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="8">
+        <v>1</v>
+      </c>
+      <c r="AK28" s="8">
         <v>1</v>
       </c>
       <c r="AL28">
@@ -4274,7 +4258,7 @@
       </c>
     </row>
     <row r="29" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B29">
@@ -4301,7 +4285,7 @@
       <c r="I29">
         <v>0</v>
       </c>
-      <c r="J29" s="11">
+      <c r="J29" s="8">
         <v>1</v>
       </c>
       <c r="K29">
@@ -4370,19 +4354,19 @@
       <c r="AF29">
         <v>0</v>
       </c>
-      <c r="AG29" s="11">
-        <v>0</v>
-      </c>
-      <c r="AH29" s="11">
-        <v>0</v>
-      </c>
-      <c r="AI29" s="11">
-        <v>0</v>
-      </c>
-      <c r="AJ29" s="11">
-        <v>1</v>
-      </c>
-      <c r="AK29" s="11">
+      <c r="AG29" s="8">
+        <v>1</v>
+      </c>
+      <c r="AH29" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI29" s="8">
+        <v>1</v>
+      </c>
+      <c r="AJ29" s="8">
+        <v>1</v>
+      </c>
+      <c r="AK29" s="8">
         <v>1</v>
       </c>
       <c r="AL29">
@@ -4402,7 +4386,7 @@
       </c>
     </row>
     <row r="30" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B30">
@@ -4429,8 +4413,8 @@
       <c r="I30">
         <v>0</v>
       </c>
-      <c r="J30" s="11">
-        <v>1</v>
+      <c r="J30">
+        <v>0</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -4498,39 +4482,39 @@
       <c r="AF30">
         <v>0</v>
       </c>
-      <c r="AG30" s="11">
-        <v>0</v>
-      </c>
-      <c r="AH30" s="11">
-        <v>0</v>
-      </c>
-      <c r="AI30" s="11">
-        <v>0</v>
-      </c>
-      <c r="AJ30" s="11">
-        <v>1</v>
-      </c>
-      <c r="AK30" s="11">
-        <v>1</v>
-      </c>
-      <c r="AL30">
-        <v>0</v>
-      </c>
-      <c r="AM30">
-        <v>0</v>
-      </c>
-      <c r="AN30">
-        <v>0</v>
-      </c>
-      <c r="AO30">
-        <v>0</v>
-      </c>
-      <c r="AP30">
-        <v>0</v>
+      <c r="AG30">
+        <v>0</v>
+      </c>
+      <c r="AH30">
+        <v>0</v>
+      </c>
+      <c r="AI30">
+        <v>0</v>
+      </c>
+      <c r="AJ30">
+        <v>0</v>
+      </c>
+      <c r="AK30">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO30" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP30" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B31">
@@ -4557,8 +4541,8 @@
       <c r="I31">
         <v>0</v>
       </c>
-      <c r="J31" s="11">
-        <v>1</v>
+      <c r="J31">
+        <v>0</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -4626,290 +4610,34 @@
       <c r="AF31">
         <v>0</v>
       </c>
-      <c r="AG31" s="11">
-        <v>1</v>
-      </c>
-      <c r="AH31" s="11">
-        <v>1</v>
-      </c>
-      <c r="AI31" s="11">
-        <v>1</v>
-      </c>
-      <c r="AJ31" s="11">
-        <v>1</v>
-      </c>
-      <c r="AK31" s="11">
-        <v>1</v>
-      </c>
-      <c r="AL31">
-        <v>0</v>
-      </c>
-      <c r="AM31">
-        <v>0</v>
-      </c>
-      <c r="AN31">
-        <v>0</v>
-      </c>
-      <c r="AO31">
-        <v>0</v>
-      </c>
-      <c r="AP31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32">
-        <v>0</v>
-      </c>
-      <c r="N32">
-        <v>0</v>
-      </c>
-      <c r="O32">
-        <v>0</v>
-      </c>
-      <c r="P32">
-        <v>0</v>
-      </c>
-      <c r="Q32">
-        <v>0</v>
-      </c>
-      <c r="R32">
-        <v>0</v>
-      </c>
-      <c r="S32">
-        <v>0</v>
-      </c>
-      <c r="T32">
-        <v>0</v>
-      </c>
-      <c r="U32">
-        <v>0</v>
-      </c>
-      <c r="V32">
-        <v>0</v>
-      </c>
-      <c r="W32">
-        <v>0</v>
-      </c>
-      <c r="X32">
-        <v>0</v>
-      </c>
-      <c r="Y32">
-        <v>0</v>
-      </c>
-      <c r="Z32">
-        <v>0</v>
-      </c>
-      <c r="AA32">
-        <v>0</v>
-      </c>
-      <c r="AB32">
-        <v>0</v>
-      </c>
-      <c r="AC32">
-        <v>0</v>
-      </c>
-      <c r="AD32">
-        <v>0</v>
-      </c>
-      <c r="AE32">
-        <v>0</v>
-      </c>
-      <c r="AF32">
-        <v>0</v>
-      </c>
-      <c r="AG32">
-        <v>0</v>
-      </c>
-      <c r="AH32">
-        <v>0</v>
-      </c>
-      <c r="AI32">
-        <v>0</v>
-      </c>
-      <c r="AJ32">
-        <v>0</v>
-      </c>
-      <c r="AK32">
-        <v>0</v>
-      </c>
-      <c r="AL32" s="12">
-        <v>1</v>
-      </c>
-      <c r="AM32" s="12">
-        <v>1</v>
-      </c>
-      <c r="AN32" s="12">
-        <v>1</v>
-      </c>
-      <c r="AO32" s="12">
-        <v>1</v>
-      </c>
-      <c r="AP32" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33">
-        <v>0</v>
-      </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
-      <c r="O33">
-        <v>0</v>
-      </c>
-      <c r="P33">
-        <v>0</v>
-      </c>
-      <c r="Q33">
-        <v>0</v>
-      </c>
-      <c r="R33">
-        <v>0</v>
-      </c>
-      <c r="S33">
-        <v>0</v>
-      </c>
-      <c r="T33">
-        <v>0</v>
-      </c>
-      <c r="U33">
-        <v>0</v>
-      </c>
-      <c r="V33">
-        <v>0</v>
-      </c>
-      <c r="W33">
-        <v>0</v>
-      </c>
-      <c r="X33">
-        <v>0</v>
-      </c>
-      <c r="Y33">
-        <v>0</v>
-      </c>
-      <c r="Z33">
-        <v>0</v>
-      </c>
-      <c r="AA33">
-        <v>0</v>
-      </c>
-      <c r="AB33">
-        <v>0</v>
-      </c>
-      <c r="AC33">
-        <v>0</v>
-      </c>
-      <c r="AD33">
-        <v>0</v>
-      </c>
-      <c r="AE33">
-        <v>0</v>
-      </c>
-      <c r="AF33">
-        <v>0</v>
-      </c>
-      <c r="AG33">
-        <v>0</v>
-      </c>
-      <c r="AH33">
-        <v>0</v>
-      </c>
-      <c r="AI33">
-        <v>0</v>
-      </c>
-      <c r="AJ33">
-        <v>0</v>
-      </c>
-      <c r="AK33">
-        <v>0</v>
-      </c>
-      <c r="AL33" s="12">
-        <v>1</v>
-      </c>
-      <c r="AM33" s="12">
-        <v>1</v>
-      </c>
-      <c r="AN33" s="12">
-        <v>1</v>
-      </c>
-      <c r="AO33" s="12">
-        <v>1</v>
-      </c>
-      <c r="AP33" s="12">
+      <c r="AG31">
+        <v>0</v>
+      </c>
+      <c r="AH31">
+        <v>0</v>
+      </c>
+      <c r="AI31">
+        <v>0</v>
+      </c>
+      <c r="AJ31">
+        <v>0</v>
+      </c>
+      <c r="AK31">
+        <v>0</v>
+      </c>
+      <c r="AL31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AM31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AO31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP31" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>